<commit_message>
new air quality data file
</commit_message>
<xml_diff>
--- a/data/Air_Quality_Data_NEW.xlsx
+++ b/data/Air_Quality_Data_NEW.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iawan\OneDrive\Documents\AirPollution-4GA3\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{415737E1-70FA-4B7B-9098-939827855C05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5392C8EB-A206-4580-87D3-6DB13FD75112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{C1991515-CDC6-4C05-917A-04B7BD49A2BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,13 +50,16 @@
     <t>PM25Avg</t>
   </si>
   <si>
+    <t>O3AVG</t>
+  </si>
+  <si>
+    <t>NO2AVG</t>
+  </si>
+  <si>
     <t>SO2AVG</t>
   </si>
   <si>
-    <t>O3AVG</t>
-  </si>
-  <si>
-    <t>NO2AVG</t>
+    <t>COAVG</t>
   </si>
   <si>
     <t>Toronto East</t>
@@ -65,6 +68,9 @@
     <t>Toronto North</t>
   </si>
   <si>
+    <t>Toronto</t>
+  </si>
+  <si>
     <t>Toronto West</t>
   </si>
   <si>
@@ -93,12 +99,6 @@
   </si>
   <si>
     <t>Harbour Terrace-1</t>
-  </si>
-  <si>
-    <t>Toronto</t>
-  </si>
-  <si>
-    <t>COAVG</t>
   </si>
   <si>
     <t>Oakwood Village Toronto</t>
@@ -115,7 +115,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -180,39 +180,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -245,9 +245,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -280,6 +297,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -341,13 +375,6 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -356,6 +383,13 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -420,27 +454,47 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBAAD5CA-0AFA-4E19-A13C-9025E08EA143}">
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="45.453125" customWidth="1"/>
+    <col min="1" max="1" width="41" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -457,21 +511,21 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
       <c r="H1" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>43.747900000000001</v>
@@ -491,7 +545,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>43.814100000000003</v>
@@ -511,7 +565,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>43.679400000000001</v>
@@ -534,7 +588,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>43.743400000000001</v>
@@ -557,7 +611,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>43.773699999999998</v>
@@ -571,7 +625,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B7">
         <v>43.659199999999998</v>
@@ -585,7 +639,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B8">
         <v>43.653599999999997</v>
@@ -599,7 +653,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B9">
         <v>43.660899999999998</v>
@@ -613,7 +667,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B10">
         <v>43.7029</v>
@@ -627,7 +681,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B11">
         <v>43.7181</v>
@@ -641,7 +695,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B12">
         <v>43.674900000000001</v>
@@ -655,7 +709,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B13">
         <v>43.626800000000003</v>
@@ -669,7 +723,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B14">
         <v>43.6372</v>
@@ -697,7 +751,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B16">
         <v>43.675699999999999</v>

</xml_diff>